<commit_message>
[#1149] isoformat context dates in spreadsheet style error tables
</commit_message>
<xml_diff>
--- a/cove_360/fixtures/badfile_all_validation_errors_4_times.xlsx
+++ b/cove_360/fixtures/badfile_all_validation_errors_4_times.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="grants" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="40">
   <si>
     <t xml:space="preserve">Identifier</t>
   </si>
@@ -60,6 +60,18 @@
   </si>
   <si>
     <t xml:space="preserve">Grant Programme:1:URL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">360G-sampletrust-105177/Z/13/Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acceptable title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acceptable description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GBP</t>
   </si>
   <si>
     <t xml:space="preserve">360G-sampletrust-105177/Z/14/Z</t>
@@ -135,8 +147,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -204,7 +217,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -215,6 +228,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -234,15 +251,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L2" activeCellId="1" sqref="10:10 L2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="9.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="1" style="0" width="9.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="9.18"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -290,146 +309,171 @@
       <c r="A2" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="0" t="n">
-        <v>9001</v>
+      <c r="B2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>15</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="L2" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="M2" s="0" t="s">
-        <v>20</v>
-      </c>
+      <c r="E2" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F2" s="3" t="n">
+        <v>43617</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>9001</v>
       </c>
       <c r="D3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="0" t="s">
+      <c r="J3" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>18</v>
+      <c r="K3" s="0" t="s">
+        <v>24</v>
       </c>
       <c r="L3" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" s="0" t="s">
         <v>24</v>
-      </c>
-      <c r="M3" s="0" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>9001</v>
       </c>
       <c r="D4" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="0" t="s">
+      <c r="G4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" s="0" t="s">
+      <c r="M4" s="0" t="s">
         <v>29</v>
-      </c>
-      <c r="K4" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="L4" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="M4" s="0" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>9001</v>
       </c>
       <c r="D5" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="0" t="s">
+      <c r="G5" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J5" s="0" t="s">
+      <c r="K5" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="K5" s="0" t="s">
+      <c r="L5" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="M5" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="L5" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="M5" s="0" t="s">
-        <v>35</v>
+      <c r="B6" s="0" t="n">
+        <v>9001</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="M6" s="0" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -450,13 +494,13 @@
   </sheetPr>
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="10:10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="9.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -472,13 +516,13 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>